<commit_message>
Monitoring and Controlling rename
</commit_message>
<xml_diff>
--- a/Concept/issue-log.xlsx
+++ b/Concept/issue-log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Testing Intake 42\QA\PMP Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\Internet-Banking-System-QA\Concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7DB113-7DCB-4382-A430-0B55170BA88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62A9687-5256-47EA-B5BF-718B3F38AFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Issue-Log'!$B$7:$C$7</definedName>
-    <definedName name="OLE_LINK1" localSheetId="0">'Issue-Log'!$M$11</definedName>
+    <definedName name="OLE_LINK1" localSheetId="0">'Issue-Log'!$O$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Issue-Log'!$3:$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -324,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -338,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -419,12 +419,6 @@
 Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Potential project cancellation or significant delay. </t>
-  </si>
-  <si>
-    <t>Logged By</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -505,19 +499,34 @@
     <t>Osama Sayed</t>
   </si>
   <si>
-    <t>Issues raised by board members about the configuration management tool and bush related to the deadline of the first release and milestone.</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
     <t>15/4/2022</t>
   </si>
   <si>
-    <t>Meet with board members to try to sovle the problem by asking them if anyone has a knowlage and can use the CM tool</t>
-  </si>
-  <si>
-    <t>One of the team members could used the tool and uploud the work berfor the deadline.</t>
+    <t xml:space="preserve">Potential project cancellation or delay. </t>
+  </si>
+  <si>
+    <t>Issues raised by board members about the configuration management tool that no one can merge on the master branch, and push the milestone related to the deadline of the first release and milestone.</t>
+  </si>
+  <si>
+    <t>Found by</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Approved by</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Meeting with board members to try to solve the problem by asking them if anyone has a knowledge about the configuration management tool and can use it.</t>
+  </si>
+  <si>
+    <t>One of the team members could use the tool and upload the work before the deadline.</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1009,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1218,9 +1227,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1233,31 +1239,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1776,10 +1788,10 @@
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL40"/>
+  <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J4" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1794,19 +1806,20 @@
     <col min="8" max="9" width="41.5546875" style="34" customWidth="1"/>
     <col min="10" max="10" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="54.109375" style="35" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="62" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39" style="60" customWidth="1"/>
-    <col min="16" max="38" width="9.109375" style="61"/>
-    <col min="39" max="16384" width="9.109375" style="3"/>
+    <col min="12" max="13" width="7.109375" style="19" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="54.109375" style="35" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39" style="60" customWidth="1"/>
+    <col min="18" max="40" width="9.109375" style="61"/>
+    <col min="41" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="74"/>
     </row>
-    <row r="2" spans="1:38" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:38" s="52" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:40" s="52" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
         <v>11</v>
       </c>
@@ -1821,16 +1834,18 @@
       <c r="J3" s="43"/>
       <c r="K3" s="41"/>
       <c r="L3" s="41"/>
-      <c r="M3" s="53"/>
-    </row>
-    <row r="4" spans="1:38" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="53"/>
+    </row>
+    <row r="4" spans="1:40" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="54" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
-      <c r="D4" s="87" t="s">
-        <v>44</v>
+      <c r="D4" s="85" t="s">
+        <v>42</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="24"/>
@@ -1840,9 +1855,9 @@
       <c r="J4" s="42"/>
       <c r="K4" s="41"/>
       <c r="L4" s="41"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="42"/>
       <c r="P4" s="59"/>
       <c r="Q4" s="59"/>
       <c r="R4" s="59"/>
@@ -1866,15 +1881,17 @@
       <c r="AJ4" s="59"/>
       <c r="AK4" s="59"/>
       <c r="AL4" s="59"/>
-    </row>
-    <row r="5" spans="1:38" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM4" s="59"/>
+      <c r="AN4" s="59"/>
+    </row>
+    <row r="5" spans="1:40" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
-      <c r="D5" s="88" t="s">
-        <v>45</v>
+      <c r="D5" s="86" t="s">
+        <v>43</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="24"/>
@@ -1884,9 +1901,9 @@
       <c r="J5" s="42"/>
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="42"/>
       <c r="P5" s="59"/>
       <c r="Q5" s="59"/>
       <c r="R5" s="59"/>
@@ -1910,8 +1927,10 @@
       <c r="AJ5" s="59"/>
       <c r="AK5" s="59"/>
       <c r="AL5" s="59"/>
-    </row>
-    <row r="6" spans="1:38" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM5" s="59"/>
+      <c r="AN5" s="59"/>
+    </row>
+    <row r="6" spans="1:40" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="55" t="s">
         <v>13</v>
       </c>
@@ -1923,12 +1942,12 @@
       <c r="G6" s="47"/>
       <c r="H6" s="47"/>
       <c r="I6" s="43"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
-      <c r="L6" s="86"/>
-      <c r="M6" s="86"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="93"/>
+      <c r="O6" s="93"/>
       <c r="P6" s="59"/>
       <c r="Q6" s="59"/>
       <c r="R6" s="59"/>
@@ -1952,8 +1971,10 @@
       <c r="AJ6" s="59"/>
       <c r="AK6" s="59"/>
       <c r="AL6" s="59"/>
-    </row>
-    <row r="7" spans="1:38" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.25">
+      <c r="AM6" s="59"/>
+      <c r="AN6" s="59"/>
+    </row>
+    <row r="7" spans="1:40" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.25">
       <c r="A7" s="68" t="s">
         <v>0</v>
       </c>
@@ -1967,13 +1988,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="72" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="70" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H7" s="70" t="s">
         <v>17</v>
@@ -1985,16 +2006,22 @@
         <v>7</v>
       </c>
       <c r="K7" s="73" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="L7" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="69" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" ht="30.6" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="M7" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="N7" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="69" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -2004,44 +2031,50 @@
       <c r="C8" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="89" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="90" t="s">
+      <c r="D8" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="91" t="s">
-        <v>48</v>
+      <c r="E8" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="89" t="s">
+        <v>45</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="92" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="93" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="94" t="s">
+      <c r="H8" s="90" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="60"/>
-      <c r="O8" s="61"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="K8" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="92" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="89" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="61"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="11"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="85"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="84"/>
       <c r="E9" s="26"/>
       <c r="F9" s="16"/>
       <c r="G9" s="21"/>
@@ -2049,12 +2082,14 @@
       <c r="I9" s="56"/>
       <c r="J9" s="16"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="61"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L9" s="95"/>
+      <c r="M9" s="95"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="61"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="13"/>
@@ -2066,12 +2101,14 @@
       <c r="I10" s="56"/>
       <c r="J10" s="16"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="61"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L10" s="95"/>
+      <c r="M10" s="95"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="61"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="11"/>
       <c r="C11" s="13"/>
@@ -2083,12 +2120,14 @@
       <c r="I11" s="38"/>
       <c r="J11" s="16"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="61"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L11" s="95"/>
+      <c r="M11" s="95"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="61"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="11"/>
       <c r="C12" s="7"/>
@@ -2100,12 +2139,14 @@
       <c r="I12" s="39"/>
       <c r="J12" s="16"/>
       <c r="K12" s="14"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="61"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="61"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13" s="7"/>
@@ -2117,12 +2158,14 @@
       <c r="I13" s="39"/>
       <c r="J13" s="16"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="61"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="61"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
@@ -2134,12 +2177,14 @@
       <c r="I14" s="39"/>
       <c r="J14" s="16"/>
       <c r="K14" s="14"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="61"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="61"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15" s="7"/>
@@ -2151,12 +2196,14 @@
       <c r="I15" s="39"/>
       <c r="J15" s="16"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="61"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="61"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="11"/>
       <c r="C16" s="7"/>
@@ -2168,12 +2215,14 @@
       <c r="I16" s="39"/>
       <c r="J16" s="16"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="61"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="61"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="11"/>
       <c r="C17" s="7"/>
@@ -2185,12 +2234,14 @@
       <c r="I17" s="39"/>
       <c r="J17" s="16"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="61"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="61"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
@@ -2202,12 +2253,14 @@
       <c r="I18" s="39"/>
       <c r="J18" s="16"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="61"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="61"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19" s="7"/>
@@ -2219,12 +2272,14 @@
       <c r="I19" s="39"/>
       <c r="J19" s="16"/>
       <c r="K19" s="14"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="61"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="61"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20" s="7"/>
@@ -2236,12 +2291,14 @@
       <c r="I20" s="39"/>
       <c r="J20" s="16"/>
       <c r="K20" s="14"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="61"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="61"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="11"/>
       <c r="C21" s="7"/>
@@ -2253,12 +2310,14 @@
       <c r="I21" s="39"/>
       <c r="J21" s="16"/>
       <c r="K21" s="14"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="61"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="61"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="11"/>
       <c r="C22" s="7"/>
@@ -2270,12 +2329,14 @@
       <c r="I22" s="39"/>
       <c r="J22" s="16"/>
       <c r="K22" s="14"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="61"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="61"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="11"/>
       <c r="C23" s="7"/>
@@ -2287,12 +2348,14 @@
       <c r="I23" s="39"/>
       <c r="J23" s="16"/>
       <c r="K23" s="14"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="61"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="61"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
@@ -2304,12 +2367,14 @@
       <c r="I24" s="39"/>
       <c r="J24" s="16"/>
       <c r="K24" s="14"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="61"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="61"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
@@ -2321,12 +2386,14 @@
       <c r="I25" s="39"/>
       <c r="J25" s="16"/>
       <c r="K25" s="14"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="61"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="61"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -2338,12 +2405,14 @@
       <c r="I26" s="39"/>
       <c r="J26" s="16"/>
       <c r="K26" s="14"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="61"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="61"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="11"/>
       <c r="C27" s="7"/>
@@ -2355,12 +2424,14 @@
       <c r="I27" s="39"/>
       <c r="J27" s="16"/>
       <c r="K27" s="14"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="60"/>
-      <c r="O27" s="61"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="61"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="11"/>
       <c r="C28" s="7"/>
@@ -2372,12 +2443,14 @@
       <c r="I28" s="39"/>
       <c r="J28" s="16"/>
       <c r="K28" s="14"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="61"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="61"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="11"/>
       <c r="C29" s="7"/>
@@ -2389,12 +2462,14 @@
       <c r="I29" s="39"/>
       <c r="J29" s="16"/>
       <c r="K29" s="14"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="61"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="61"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="11"/>
       <c r="C30" s="7"/>
@@ -2406,12 +2481,14 @@
       <c r="I30" s="39"/>
       <c r="J30" s="16"/>
       <c r="K30" s="14"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="61"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="61"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="11"/>
       <c r="C31" s="7"/>
@@ -2423,12 +2500,14 @@
       <c r="I31" s="39"/>
       <c r="J31" s="16"/>
       <c r="K31" s="14"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="61"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="61"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="11"/>
       <c r="C32" s="7"/>
@@ -2440,12 +2519,14 @@
       <c r="I32" s="39"/>
       <c r="J32" s="16"/>
       <c r="K32" s="14"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="61"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="61"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="11"/>
       <c r="C33" s="7"/>
@@ -2457,12 +2538,14 @@
       <c r="I33" s="39"/>
       <c r="J33" s="16"/>
       <c r="K33" s="14"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="61"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="31"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="61"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="11"/>
       <c r="C34" s="7"/>
@@ -2474,12 +2557,14 @@
       <c r="I34" s="39"/>
       <c r="J34" s="16"/>
       <c r="K34" s="14"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="60"/>
-      <c r="O34" s="61"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="61"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="11"/>
       <c r="C35" s="7"/>
@@ -2491,12 +2576,14 @@
       <c r="I35" s="39"/>
       <c r="J35" s="16"/>
       <c r="K35" s="14"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="60"/>
-      <c r="O35" s="61"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="61"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="11"/>
       <c r="C36" s="7"/>
@@ -2508,12 +2595,14 @@
       <c r="I36" s="39"/>
       <c r="J36" s="16"/>
       <c r="K36" s="14"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="61"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="61"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="11"/>
       <c r="C37" s="7"/>
@@ -2525,12 +2614,14 @@
       <c r="I37" s="39"/>
       <c r="J37" s="16"/>
       <c r="K37" s="14"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="31"/>
-      <c r="N37" s="60"/>
-      <c r="O37" s="61"/>
-    </row>
-    <row r="38" spans="1:15" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="61"/>
+    </row>
+    <row r="38" spans="1:17" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="12"/>
       <c r="C38" s="10"/>
@@ -2542,17 +2633,19 @@
       <c r="I38" s="40"/>
       <c r="J38" s="18"/>
       <c r="K38" s="17"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="60"/>
-      <c r="O38" s="61"/>
-    </row>
-    <row r="40" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="61"/>
+    </row>
+    <row r="40" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="D40" s="75" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E40" s="76" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F40" s="77"/>
       <c r="G40" s="77"/>
@@ -2563,7 +2656,7 @@
   </sheetData>
   <autoFilter ref="B7:C7" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J6:O6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="J39:J65538 J3 C3 C7:C65538 B7:B38">
@@ -2580,7 +2673,7 @@
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3 G7:G38 K4:K5">
+  <conditionalFormatting sqref="N3 G7:G38 K4:M5">
     <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2628,10 +2721,10 @@
     <row r="1" spans="2:3" ht="80.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B3" s="65" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="65" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2639,7 +2732,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2647,7 +2740,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2655,7 +2748,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="67" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2663,15 +2756,15 @@
         <v>6</v>
       </c>
       <c r="C7" s="67" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="18" x14ac:dyDescent="0.35">
       <c r="C24" s="75" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D24" s="76" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2702,10 +2795,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B2:B9"/>
+  <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2714,55 +2807,100 @@
     <col min="2" max="16384" width="9.109375" style="78"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="80" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="81" t="s">
+    <row r="2" spans="1:8" s="79" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B2" s="80" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+    </row>
+    <row r="4" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="94" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" s="80" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="79" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+    </row>
+    <row r="5" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+    </row>
+    <row r="6" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="94" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" s="80" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="79" t="s">
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+    </row>
+    <row r="7" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="94" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" s="80" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="79" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" s="80" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="79" t="s">
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+    </row>
+    <row r="8" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="94" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" s="80" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="79" t="s">
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+    </row>
+    <row r="9" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="94" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" s="80" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="79" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" s="80" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="79" t="s">
-        <v>39</v>
-      </c>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{7FA5BDE0-1CDC-44BC-A10F-9C6FF06BDA02}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{21C008BE-2783-45CE-9493-FC5893211F59}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{F68A8FA3-5AF3-46CD-80E2-CC2427D98263}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{5F48E782-0877-4CF7-8533-264E68F6BDC4}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{1010D7A3-542A-490E-B360-F02240317C1E}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{21C008BE-2783-45CE-9493-FC5893211F59}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{F68A8FA3-5AF3-46CD-80E2-CC2427D98263}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{5F48E782-0877-4CF7-8533-264E68F6BDC4}"/>
+    <hyperlink ref="A9" r:id="rId5" xr:uid="{1010D7A3-542A-490E-B360-F02240317C1E}"/>
     <hyperlink ref="B4" r:id="rId6" xr:uid="{43F7D3DA-9797-41B3-A587-A174EEFA4CEB}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{97619E3A-DD0B-4AF3-9BA5-EDFFF3715870}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{97619E3A-DD0B-4AF3-9BA5-EDFFF3715870}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2779,31 +2917,31 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="83" t="s">
+      <c r="A1" s="81" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="82" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:1" s="83" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Concept & revews update
</commit_message>
<xml_diff>
--- a/Concept/issue-log.xlsx
+++ b/Concept/issue-log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ossay\Downloads\New folder\Internet-Banking-System-QA\Concept\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62A9687-5256-47EA-B5BF-718B3F38AFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169A9151-CBB0-4A77-886B-025B9B43D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Issue-Log" sheetId="2" r:id="rId1"/>
@@ -1263,14 +1263,14 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1790,36 +1790,36 @@
   </sheetPr>
   <dimension ref="A1:AN40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5546875" style="34" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="34" customWidth="1"/>
     <col min="5" max="5" width="11" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="34" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="34" customWidth="1"/>
-    <col min="8" max="9" width="41.5546875" style="34" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.109375" style="19" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="54.109375" style="35" customWidth="1"/>
-    <col min="16" max="16" width="9.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="34" customWidth="1"/>
+    <col min="8" max="9" width="41.5703125" style="34" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.140625" style="19" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="54.140625" style="35" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" style="62" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="39" style="60" customWidth="1"/>
-    <col min="18" max="40" width="9.109375" style="61"/>
-    <col min="41" max="16384" width="9.109375" style="3"/>
+    <col min="18" max="40" width="9.140625" style="61"/>
+    <col min="41" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="74"/>
     </row>
-    <row r="2" spans="1:40" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:40" s="52" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:40" s="52" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>11</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="N3" s="41"/>
       <c r="O3" s="53"/>
     </row>
-    <row r="4" spans="1:40" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
         <v>8</v>
       </c>
@@ -1884,7 +1884,7 @@
       <c r="AM4" s="59"/>
       <c r="AN4" s="59"/>
     </row>
-    <row r="5" spans="1:40" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>9</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="AM5" s="59"/>
       <c r="AN5" s="59"/>
     </row>
-    <row r="6" spans="1:40" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="55" t="s">
         <v>13</v>
       </c>
@@ -1942,12 +1942,12 @@
       <c r="G6" s="47"/>
       <c r="H6" s="47"/>
       <c r="I6" s="43"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="93"/>
-      <c r="N6" s="93"/>
-      <c r="O6" s="93"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
       <c r="P6" s="59"/>
       <c r="Q6" s="59"/>
       <c r="R6" s="59"/>
@@ -1974,7 +1974,7 @@
       <c r="AM6" s="59"/>
       <c r="AN6" s="59"/>
     </row>
-    <row r="7" spans="1:40" s="2" customFormat="1" ht="69" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:40" ht="40.799999999999997" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -2070,7 +2070,7 @@
       <c r="P8" s="60"/>
       <c r="Q8" s="61"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="11"/>
       <c r="C9" s="83"/>
@@ -2082,14 +2082,14 @@
       <c r="I9" s="56"/>
       <c r="J9" s="16"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="93"/>
       <c r="N9" s="15"/>
       <c r="O9" s="27"/>
       <c r="P9" s="60"/>
       <c r="Q9" s="61"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="13"/>
@@ -2101,14 +2101,14 @@
       <c r="I10" s="56"/>
       <c r="J10" s="16"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="95"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
       <c r="N10" s="15"/>
       <c r="O10" s="27"/>
       <c r="P10" s="60"/>
       <c r="Q10" s="61"/>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="11"/>
       <c r="C11" s="13"/>
@@ -2120,14 +2120,14 @@
       <c r="I11" s="38"/>
       <c r="J11" s="16"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="95"/>
-      <c r="M11" s="95"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
       <c r="N11" s="15"/>
       <c r="O11" s="27"/>
       <c r="P11" s="60"/>
       <c r="Q11" s="61"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="11"/>
       <c r="C12" s="7"/>
@@ -2146,7 +2146,7 @@
       <c r="P12" s="60"/>
       <c r="Q12" s="61"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="11"/>
       <c r="C13" s="7"/>
@@ -2165,7 +2165,7 @@
       <c r="P13" s="60"/>
       <c r="Q13" s="61"/>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="11"/>
       <c r="C14" s="7"/>
@@ -2184,7 +2184,7 @@
       <c r="P14" s="60"/>
       <c r="Q14" s="61"/>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="11"/>
       <c r="C15" s="7"/>
@@ -2203,7 +2203,7 @@
       <c r="P15" s="60"/>
       <c r="Q15" s="61"/>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="11"/>
       <c r="C16" s="7"/>
@@ -2222,7 +2222,7 @@
       <c r="P16" s="60"/>
       <c r="Q16" s="61"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="11"/>
       <c r="C17" s="7"/>
@@ -2241,7 +2241,7 @@
       <c r="P17" s="60"/>
       <c r="Q17" s="61"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="11"/>
       <c r="C18" s="7"/>
@@ -2260,7 +2260,7 @@
       <c r="P18" s="60"/>
       <c r="Q18" s="61"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="11"/>
       <c r="C19" s="7"/>
@@ -2279,7 +2279,7 @@
       <c r="P19" s="60"/>
       <c r="Q19" s="61"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="11"/>
       <c r="C20" s="7"/>
@@ -2298,7 +2298,7 @@
       <c r="P20" s="60"/>
       <c r="Q20" s="61"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="11"/>
       <c r="C21" s="7"/>
@@ -2317,7 +2317,7 @@
       <c r="P21" s="60"/>
       <c r="Q21" s="61"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="11"/>
       <c r="C22" s="7"/>
@@ -2336,7 +2336,7 @@
       <c r="P22" s="60"/>
       <c r="Q22" s="61"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="11"/>
       <c r="C23" s="7"/>
@@ -2355,7 +2355,7 @@
       <c r="P23" s="60"/>
       <c r="Q23" s="61"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="11"/>
       <c r="C24" s="7"/>
@@ -2374,7 +2374,7 @@
       <c r="P24" s="60"/>
       <c r="Q24" s="61"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="11"/>
       <c r="C25" s="7"/>
@@ -2393,7 +2393,7 @@
       <c r="P25" s="60"/>
       <c r="Q25" s="61"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="11"/>
       <c r="C26" s="7"/>
@@ -2412,7 +2412,7 @@
       <c r="P26" s="60"/>
       <c r="Q26" s="61"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="11"/>
       <c r="C27" s="7"/>
@@ -2431,7 +2431,7 @@
       <c r="P27" s="60"/>
       <c r="Q27" s="61"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="11"/>
       <c r="C28" s="7"/>
@@ -2450,7 +2450,7 @@
       <c r="P28" s="60"/>
       <c r="Q28" s="61"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="11"/>
       <c r="C29" s="7"/>
@@ -2469,7 +2469,7 @@
       <c r="P29" s="60"/>
       <c r="Q29" s="61"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="11"/>
       <c r="C30" s="7"/>
@@ -2488,7 +2488,7 @@
       <c r="P30" s="60"/>
       <c r="Q30" s="61"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="11"/>
       <c r="C31" s="7"/>
@@ -2507,7 +2507,7 @@
       <c r="P31" s="60"/>
       <c r="Q31" s="61"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="11"/>
       <c r="C32" s="7"/>
@@ -2526,7 +2526,7 @@
       <c r="P32" s="60"/>
       <c r="Q32" s="61"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="11"/>
       <c r="C33" s="7"/>
@@ -2545,7 +2545,7 @@
       <c r="P33" s="60"/>
       <c r="Q33" s="61"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
       <c r="B34" s="11"/>
       <c r="C34" s="7"/>
@@ -2564,7 +2564,7 @@
       <c r="P34" s="60"/>
       <c r="Q34" s="61"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="11"/>
       <c r="C35" s="7"/>
@@ -2583,7 +2583,7 @@
       <c r="P35" s="60"/>
       <c r="Q35" s="61"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="11"/>
       <c r="C36" s="7"/>
@@ -2602,7 +2602,7 @@
       <c r="P36" s="60"/>
       <c r="Q36" s="61"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="11"/>
       <c r="C37" s="7"/>
@@ -2621,7 +2621,7 @@
       <c r="P37" s="60"/>
       <c r="Q37" s="61"/>
     </row>
-    <row r="38" spans="1:17" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="12"/>
       <c r="C38" s="10"/>
@@ -2640,7 +2640,7 @@
       <c r="P38" s="60"/>
       <c r="Q38" s="61"/>
     </row>
-    <row r="40" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D40" s="75" t="s">
         <v>29</v>
       </c>
@@ -2710,16 +2710,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="63"/>
-    <col min="2" max="2" width="18.33203125" style="63" customWidth="1"/>
-    <col min="3" max="3" width="49.6640625" style="63" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="63"/>
+    <col min="1" max="1" width="9.140625" style="63"/>
+    <col min="2" max="2" width="18.28515625" style="63" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="63" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="80.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" ht="80.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B3" s="65" t="s">
         <v>24</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="64" t="s">
         <v>12</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="64" t="s">
         <v>3</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="64" t="s">
         <v>4</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="64" t="s">
         <v>6</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="3:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C24" s="75" t="s">
         <v>29</v>
       </c>
@@ -2801,87 +2801,87 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="78" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="78"/>
+    <col min="1" max="1" width="4.28515625" style="78" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="78"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="79" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="79" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="80" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="94" t="s">
+    <row r="3" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-    </row>
-    <row r="4" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="94" t="s">
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+    </row>
+    <row r="4" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-    </row>
-    <row r="5" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="94" t="s">
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+    </row>
+    <row r="5" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-    </row>
-    <row r="6" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+    </row>
+    <row r="6" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
-    </row>
-    <row r="7" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="94" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+    </row>
+    <row r="7" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-    </row>
-    <row r="8" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+    </row>
+    <row r="8" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-    </row>
-    <row r="9" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="94" t="s">
+      <c r="B8" s="95"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="95"/>
+    </row>
+    <row r="9" spans="1:8" s="79" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2914,34 +2914,34 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="81" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="82" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="82" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:1" s="82" customFormat="1" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:1" s="82" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>